<commit_message>
More improvements in excel connector
</commit_message>
<xml_diff>
--- a/tst/Encamina.Enmarcha.SemanticKernel.Connectors.Document.Tests/TestUtilities/Files/TestFileWithFormatValues.xlsx
+++ b/tst/Encamina.Enmarcha.SemanticKernel.Connectors.Document.Tests/TestUtilities/Files/TestFileWithFormatValues.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmarcos\OneDrive - ENCAMINA S.L\Documentos\GitHub\enmarcha\tst\Encamina.Enmarcha.SemanticKernel.Connectors.Document.Tests\TestUtilities\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmarcos\OneDrive - ENCAMINA S.L\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34108BF-9F4A-4D6C-A0FE-31F90840B9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993EE19D-00A3-42E7-945E-7E02DB4B47AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="2850" windowWidth="29040" windowHeight="15720" xr2:uid="{CDF9DF9E-DD88-401C-A97F-19EEC9BC2079}"/>
   </bookViews>
@@ -37,9 +37,9 @@
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="#,##0.0\ ;\(#,##0.0\);\-"/>
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="170" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="169" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="174" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -98,13 +98,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +423,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,5 +478,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>